<commit_message>
Added code to print out words associated with each DoD
</commit_message>
<xml_diff>
--- a/logReg_coef_expGroup.xlsx
+++ b/logReg_coef_expGroup.xlsx
@@ -55,264 +55,264 @@
     <t>personal</t>
   </si>
   <si>
+    <t>disruptive</t>
+  </si>
+  <si>
+    <t>strife</t>
+  </si>
+  <si>
+    <t>long term</t>
+  </si>
+  <si>
+    <t>irreversible</t>
+  </si>
+  <si>
+    <t>nonpartisan</t>
+  </si>
+  <si>
+    <t>economic prosperity</t>
+  </si>
+  <si>
+    <t>cautious approach</t>
+  </si>
+  <si>
+    <t>consequence</t>
+  </si>
+  <si>
+    <t>footprint</t>
+  </si>
+  <si>
+    <t>reliable energy</t>
+  </si>
+  <si>
+    <t>impossible</t>
+  </si>
+  <si>
+    <t>total emissions</t>
+  </si>
+  <si>
+    <t>invent</t>
+  </si>
+  <si>
+    <t>take advantage</t>
+  </si>
+  <si>
+    <t>unavoidable</t>
+  </si>
+  <si>
+    <t>hinder</t>
+  </si>
+  <si>
     <t>commitment</t>
   </si>
   <si>
+    <t>inevitable</t>
+  </si>
+  <si>
+    <t>exploited</t>
+  </si>
+  <si>
+    <t>fate</t>
+  </si>
+  <si>
+    <t>lowincome</t>
+  </si>
+  <si>
+    <t>adapt</t>
+  </si>
+  <si>
+    <t>overuse</t>
+  </si>
+  <si>
+    <t>cleaner fuels</t>
+  </si>
+  <si>
+    <t>doubt</t>
+  </si>
+  <si>
+    <t>catastrophe</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>promised</t>
+  </si>
+  <si>
+    <t>mutually beneficial</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>unimaginable</t>
+  </si>
+  <si>
+    <t>breakthrough</t>
+  </si>
+  <si>
+    <t>exploit</t>
+  </si>
+  <si>
+    <t>ambition</t>
+  </si>
+  <si>
+    <t>overburdened</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>best interest</t>
+  </si>
+  <si>
+    <t>appetite</t>
+  </si>
+  <si>
+    <t>compromise</t>
+  </si>
+  <si>
+    <t>tragedy commons</t>
+  </si>
+  <si>
+    <t>consumer choice</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>living standards</t>
+  </si>
+  <si>
+    <t>low carbon</t>
+  </si>
+  <si>
+    <t>sequestration</t>
+  </si>
+  <si>
+    <t>burden</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>fusion</t>
+  </si>
+  <si>
+    <t>renewable natural</t>
+  </si>
+  <si>
+    <t>regressive</t>
+  </si>
+  <si>
+    <t>voluntary</t>
+  </si>
+  <si>
+    <t>lower carbon</t>
+  </si>
+  <si>
+    <t>adaptation</t>
+  </si>
+  <si>
+    <t>sacrifice</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>compete</t>
+  </si>
+  <si>
+    <t>rush</t>
+  </si>
+  <si>
+    <t>insurmountable</t>
+  </si>
+  <si>
+    <t>grim</t>
+  </si>
+  <si>
+    <t>disproportionate</t>
+  </si>
+  <si>
     <t>near future</t>
   </si>
   <si>
+    <t>marketplace</t>
+  </si>
+  <si>
     <t>resignation</t>
   </si>
   <si>
-    <t>promised</t>
-  </si>
-  <si>
-    <t>fear</t>
-  </si>
-  <si>
-    <t>fate</t>
-  </si>
-  <si>
-    <t>cleaner fuels</t>
+    <t>prescribe</t>
+  </si>
+  <si>
+    <t>promise</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>costly</t>
+  </si>
+  <si>
+    <t>disruption</t>
+  </si>
+  <si>
+    <t>infeasible</t>
+  </si>
+  <si>
+    <t>negligible</t>
+  </si>
+  <si>
+    <t>affordable</t>
+  </si>
+  <si>
+    <t>overused</t>
+  </si>
+  <si>
+    <t>socioeconomic</t>
+  </si>
+  <si>
+    <t>uncertainty</t>
+  </si>
+  <si>
+    <t>incentive</t>
+  </si>
+  <si>
+    <t>unequivocal</t>
+  </si>
+  <si>
+    <t>energy needs</t>
+  </si>
+  <si>
+    <t>energy management</t>
+  </si>
+  <si>
+    <t>imminent</t>
+  </si>
+  <si>
+    <t>carbon intensity</t>
+  </si>
+  <si>
+    <t>carbon footprint</t>
+  </si>
+  <si>
+    <t>research development</t>
   </si>
   <si>
     <t>invest</t>
   </si>
   <si>
-    <t>research development</t>
-  </si>
-  <si>
-    <t>reliable energy</t>
-  </si>
-  <si>
-    <t>socioeconomic</t>
+    <t>low income</t>
+  </si>
+  <si>
+    <t>exploiting</t>
   </si>
   <si>
     <t>unfair</t>
   </si>
   <si>
-    <t>appetite</t>
-  </si>
-  <si>
-    <t>prescribe</t>
-  </si>
-  <si>
-    <t>burden</t>
-  </si>
-  <si>
-    <t>compete</t>
-  </si>
-  <si>
-    <t>doubt</t>
-  </si>
-  <si>
-    <t>sacrifice</t>
-  </si>
-  <si>
-    <t>incentive</t>
-  </si>
-  <si>
-    <t>negligible</t>
-  </si>
-  <si>
-    <t>carbon footprint</t>
-  </si>
-  <si>
-    <t>competition</t>
-  </si>
-  <si>
-    <t>regressive</t>
-  </si>
-  <si>
-    <t>marketplace</t>
-  </si>
-  <si>
-    <t>lowincome</t>
-  </si>
-  <si>
-    <t>costly</t>
-  </si>
-  <si>
-    <t>infeasible</t>
-  </si>
-  <si>
-    <t>grim</t>
-  </si>
-  <si>
-    <t>energy management</t>
-  </si>
-  <si>
-    <t>imminent</t>
-  </si>
-  <si>
-    <t>carbon intensity</t>
-  </si>
-  <si>
-    <t>footprint</t>
-  </si>
-  <si>
-    <t>irreversible</t>
-  </si>
-  <si>
-    <t>promise</t>
-  </si>
-  <si>
-    <t>living standards</t>
-  </si>
-  <si>
-    <t>impossible</t>
-  </si>
-  <si>
-    <t>overuse</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>unequivocal</t>
-  </si>
-  <si>
-    <t>disproportionate</t>
-  </si>
-  <si>
-    <t>exploited</t>
-  </si>
-  <si>
-    <t>rush</t>
-  </si>
-  <si>
-    <t>sequestration</t>
-  </si>
-  <si>
-    <t>creator</t>
-  </si>
-  <si>
-    <t>consequence</t>
-  </si>
-  <si>
-    <t>consumer choice</t>
-  </si>
-  <si>
-    <t>disruptive</t>
-  </si>
-  <si>
-    <t>disruption</t>
-  </si>
-  <si>
-    <t>natural gas</t>
-  </si>
-  <si>
-    <t>mutually beneficial</t>
-  </si>
-  <si>
-    <t>overburdened</t>
-  </si>
-  <si>
-    <t>ambition</t>
-  </si>
-  <si>
-    <t>take advantage</t>
-  </si>
-  <si>
-    <t>fusion</t>
-  </si>
-  <si>
-    <t>shared</t>
-  </si>
-  <si>
-    <t>compromise</t>
-  </si>
-  <si>
-    <t>adaptation</t>
-  </si>
-  <si>
-    <t>breakthrough</t>
-  </si>
-  <si>
-    <t>adapt</t>
-  </si>
-  <si>
-    <t>exploiting</t>
-  </si>
-  <si>
-    <t>strife</t>
-  </si>
-  <si>
-    <t>nonpartisan</t>
-  </si>
-  <si>
-    <t>invent</t>
-  </si>
-  <si>
-    <t>unimaginable</t>
-  </si>
-  <si>
-    <t>cautious approach</t>
-  </si>
-  <si>
-    <t>unavoidable</t>
-  </si>
-  <si>
-    <t>insurmountable</t>
-  </si>
-  <si>
-    <t>low income</t>
-  </si>
-  <si>
-    <t>long term</t>
-  </si>
-  <si>
-    <t>catastrophe</t>
-  </si>
-  <si>
-    <t>poor</t>
-  </si>
-  <si>
-    <t>exploit</t>
-  </si>
-  <si>
-    <t>tragedy commons</t>
-  </si>
-  <si>
-    <t>lower carbon</t>
-  </si>
-  <si>
-    <t>economic prosperity</t>
-  </si>
-  <si>
-    <t>overused</t>
-  </si>
-  <si>
-    <t>total emissions</t>
-  </si>
-  <si>
-    <t>inevitable</t>
-  </si>
-  <si>
-    <t>renewable natural</t>
-  </si>
-  <si>
-    <t>low carbon</t>
-  </si>
-  <si>
-    <t>best interest</t>
-  </si>
-  <si>
-    <t>affordable</t>
-  </si>
-  <si>
-    <t>hinder</t>
-  </si>
-  <si>
-    <t>uncertainty</t>
-  </si>
-  <si>
-    <t>voluntary</t>
-  </si>
-  <si>
-    <t>energy needs</t>
-  </si>
-  <si>
     <t>inflation</t>
   </si>
   <si>
@@ -361,31 +361,31 @@
     <t>{'Tech_optimism'}</t>
   </si>
   <si>
+    <t>{'Social_justice'}</t>
+  </si>
+  <si>
+    <t>{'Perfect_policy'}</t>
+  </si>
+  <si>
     <t>{'FF_solutionism'}</t>
   </si>
   <si>
-    <t>{'Social_justice'}</t>
-  </si>
-  <si>
     <t>{'Whataboutism'}</t>
   </si>
   <si>
+    <t>{'Free_rider'}</t>
+  </si>
+  <si>
     <t>{'Carrots'}</t>
   </si>
   <si>
-    <t>{'Social_justice', 'Carrots', 'Free_rider'}</t>
-  </si>
-  <si>
-    <t>{'Free_rider'}</t>
-  </si>
-  <si>
-    <t>{'Perfect_policy'}</t>
-  </si>
-  <si>
-    <t>{'Carrots', 'Free_rider'}</t>
+    <t>{'Free_rider', 'Carrots'}</t>
   </si>
   <si>
     <t>{'Social_justice', 'Well_being'}</t>
+  </si>
+  <si>
+    <t>{'Free_rider', 'Social_justice', 'Carrots'}</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.4432336313258494</v>
+        <v>-0.4432308849471093</v>
       </c>
       <c r="C2" t="s">
         <v>109</v>
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-0.4424092316056566</v>
+        <v>-0.4424047452443152</v>
       </c>
       <c r="C3" t="s">
         <v>110</v>
@@ -796,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.4420544794894407</v>
+        <v>-0.4420555844738485</v>
       </c>
       <c r="C4" t="s">
         <v>110</v>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-0.3887658360782781</v>
+        <v>-0.3887660374665793</v>
       </c>
       <c r="C5" t="s">
         <v>111</v>
@@ -824,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-0.2692527474591727</v>
+        <v>-0.2692515226563703</v>
       </c>
       <c r="C6" t="s">
         <v>110</v>
@@ -838,7 +838,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.1876400635832342</v>
+        <v>-0.1876325729197048</v>
       </c>
       <c r="C7" t="s">
         <v>112</v>
@@ -852,7 +852,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.1477354781038601</v>
+        <v>-0.1477319125161749</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
@@ -866,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-0.08532811490612763</v>
+        <v>-0.08532454921840424</v>
       </c>
       <c r="C9" t="s">
         <v>114</v>
@@ -880,7 +880,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>-0.02479988308938715</v>
+        <v>-0.02479582550875902</v>
       </c>
       <c r="C10" t="s">
         <v>111</v>
@@ -897,10 +897,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D11">
-        <v>629</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -911,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -925,10 +925,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -939,10 +939,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D14">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -953,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D15">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -967,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -981,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -995,10 +995,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D18">
-        <v>151</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1037,10 +1037,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1051,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1065,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1079,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1093,10 +1093,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D25">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1107,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D26">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27">
-        <v>35</v>
+        <v>629</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1135,10 +1135,10 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D28">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1149,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D29">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1163,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1177,10 +1177,10 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31">
-        <v>21</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1191,10 +1191,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D32">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1205,10 +1205,10 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1219,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1233,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D35">
-        <v>101</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D36">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1261,10 +1261,10 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1275,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D38">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1289,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D39">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1303,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1317,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1331,10 +1331,10 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D42">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1345,10 +1345,10 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D43">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1362,7 +1362,7 @@
         <v>110</v>
       </c>
       <c r="D44">
-        <v>93</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1373,10 +1373,10 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1387,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D46">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1401,10 +1401,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D47">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1415,10 +1415,10 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D48">
-        <v>136</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1429,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1443,10 +1443,10 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D50">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1457,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D52">
-        <v>38</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1485,10 +1485,10 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D53">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1499,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D54">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1513,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D55">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1527,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D56">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1541,10 +1541,10 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D57">
-        <v>11</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1555,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D58">
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1569,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D59">
-        <v>105</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1583,10 +1583,10 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D60">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1597,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1611,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D62">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1625,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D63">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1639,10 +1639,10 @@
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D65">
         <v>229</v>
@@ -1667,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D66">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D67">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1695,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D68">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1712,7 +1712,7 @@
         <v>113</v>
       </c>
       <c r="D69">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1723,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D70">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1737,10 +1737,10 @@
         <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1751,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D72">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1765,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D73">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1779,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D74">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1793,10 +1793,10 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1810,7 +1810,7 @@
         <v>113</v>
       </c>
       <c r="D76">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1821,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1835,10 +1835,10 @@
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D78">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D79">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1863,10 +1863,10 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D80">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1877,10 +1877,10 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D81">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1891,10 +1891,10 @@
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D82">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1905,10 +1905,10 @@
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1919,10 +1919,10 @@
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D84">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1933,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D85">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1947,10 +1947,10 @@
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1961,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D87">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1975,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D88">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1989,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2003,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D90">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2017,10 +2017,10 @@
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2031,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D92">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2045,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2059,10 +2059,10 @@
         <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D94">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2073,10 +2073,10 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D95">
-        <v>79</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2087,10 +2087,10 @@
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D96">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2101,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -2112,7 +2112,7 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>0.0110678911774367</v>
+        <v>0.01107190747934587</v>
       </c>
       <c r="C98" t="s">
         <v>112</v>
@@ -2126,7 +2126,7 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>0.1611338264212</v>
+        <v>0.161138764811037</v>
       </c>
       <c r="C99" t="s">
         <v>112</v>
@@ -2140,10 +2140,10 @@
         <v>102</v>
       </c>
       <c r="B100">
-        <v>0.2100798283060975</v>
+        <v>0.2100830696858814</v>
       </c>
       <c r="C100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D100">
         <v>396</v>
@@ -2154,10 +2154,10 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>0.2180180980186087</v>
+        <v>0.2180173262150243</v>
       </c>
       <c r="C101" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D101">
         <v>75</v>
@@ -2168,7 +2168,7 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>0.2337379516245505</v>
+        <v>0.2337368045715202</v>
       </c>
       <c r="C102" t="s">
         <v>114</v>
@@ -2182,7 +2182,7 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>0.3644170984549766</v>
+        <v>0.3644207134070223</v>
       </c>
       <c r="C103" t="s">
         <v>114</v>
@@ -2196,10 +2196,10 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>0.4856359532762173</v>
+        <v>0.485639571212969</v>
       </c>
       <c r="C104" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D104">
         <v>304</v>
@@ -2210,10 +2210,10 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>0.60784756199667</v>
+        <v>0.6078495832189693</v>
       </c>
       <c r="C105" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D105">
         <v>107</v>
@@ -2224,10 +2224,10 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>1.207534317306971</v>
+        <v>1.207540724375152</v>
       </c>
       <c r="C106" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D106">
         <v>227</v>

</xml_diff>

<commit_message>
Made Rachel's edits to regressions
</commit_message>
<xml_diff>
--- a/logReg_coef_expGroup.xlsx
+++ b/logReg_coef_expGroup.xlsx
@@ -19,7 +19,7 @@
     <t>var</t>
   </si>
   <si>
-    <t>val_logitlasso</t>
+    <t>val_lasso</t>
   </si>
   <si>
     <t>DoD_Dicts</t>
@@ -28,364 +28,364 @@
     <t>wordCount</t>
   </si>
   <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>unavoidable</t>
+  </si>
+  <si>
+    <t>breakthrough</t>
+  </si>
+  <si>
+    <t>overuse</t>
+  </si>
+  <si>
+    <t>invent</t>
+  </si>
+  <si>
+    <t>disproportionate</t>
+  </si>
+  <si>
+    <t>volunteer</t>
+  </si>
+  <si>
+    <t>uncertainty</t>
+  </si>
+  <si>
+    <t>living standards</t>
+  </si>
+  <si>
+    <t>marketplace</t>
+  </si>
+  <si>
+    <t>catastrophe</t>
+  </si>
+  <si>
+    <t>mutually beneficial</t>
+  </si>
+  <si>
+    <t>infeasible</t>
+  </si>
+  <si>
+    <t>low income</t>
+  </si>
+  <si>
+    <t>compete</t>
+  </si>
+  <si>
+    <t>socioeconomic</t>
+  </si>
+  <si>
+    <t>compromise</t>
+  </si>
+  <si>
+    <t>long term</t>
+  </si>
+  <si>
+    <t>overused</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>carbon footprint</t>
+  </si>
+  <si>
+    <t>energy needs</t>
+  </si>
+  <si>
+    <t>sequestration</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>commitment</t>
+  </si>
+  <si>
+    <t>reliable energy</t>
+  </si>
+  <si>
+    <t>disruption</t>
+  </si>
+  <si>
+    <t>overburdened</t>
+  </si>
+  <si>
+    <t>renewable natural</t>
+  </si>
+  <si>
+    <t>footprint</t>
+  </si>
+  <si>
+    <t>promised</t>
+  </si>
+  <si>
+    <t>private sector</t>
+  </si>
+  <si>
+    <t>take advantage</t>
+  </si>
+  <si>
+    <t>cautious approach</t>
+  </si>
+  <si>
+    <t>incentive</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>carbon intensity</t>
+  </si>
+  <si>
+    <t>energy management</t>
+  </si>
+  <si>
+    <t>innovation</t>
+  </si>
+  <si>
+    <t>prescribe</t>
+  </si>
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>affordable</t>
+  </si>
+  <si>
+    <t>incentives</t>
+  </si>
+  <si>
+    <t>ambition</t>
+  </si>
+  <si>
+    <t>lowincome</t>
+  </si>
+  <si>
+    <t>exploit</t>
+  </si>
+  <si>
+    <t>grim</t>
+  </si>
+  <si>
+    <t>bipartisan</t>
+  </si>
+  <si>
+    <t>total emissions</t>
+  </si>
+  <si>
+    <t>regressive</t>
+  </si>
+  <si>
+    <t>negligible</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>consequence</t>
+  </si>
+  <si>
+    <t>costly</t>
+  </si>
+  <si>
     <t>failure</t>
   </si>
   <si>
+    <t>extreme</t>
+  </si>
+  <si>
+    <t>impossible</t>
+  </si>
+  <si>
+    <t>tragedy commons</t>
+  </si>
+  <si>
+    <t>unfair</t>
+  </si>
+  <si>
+    <t>nonpartisan</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>strife</t>
+  </si>
+  <si>
+    <t>fusion</t>
+  </si>
+  <si>
+    <t>best interest</t>
+  </si>
+  <si>
+    <t>sacrifice</t>
+  </si>
+  <si>
+    <t>committed</t>
+  </si>
+  <si>
     <t>promises</t>
   </si>
   <si>
+    <t>burden</t>
+  </si>
+  <si>
+    <t>hinder</t>
+  </si>
+  <si>
+    <t>vulnerable</t>
+  </si>
+  <si>
+    <t>fate</t>
+  </si>
+  <si>
+    <t>exploiting</t>
+  </si>
+  <si>
     <t>commitments</t>
   </si>
   <si>
+    <t>irreversible</t>
+  </si>
+  <si>
+    <t>appetite</t>
+  </si>
+  <si>
+    <t>unimaginable</t>
+  </si>
+  <si>
+    <t>threat</t>
+  </si>
+  <si>
+    <t>consumer choice</t>
+  </si>
+  <si>
+    <t>promise</t>
+  </si>
+  <si>
+    <t>voluntary</t>
+  </si>
+  <si>
+    <t>adapt</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>insurmountable</t>
+  </si>
+  <si>
+    <t>exploited</t>
+  </si>
+  <si>
+    <t>research development</t>
+  </si>
+  <si>
+    <t>economic prosperity</t>
+  </si>
+  <si>
+    <t>cleaner fuels</t>
+  </si>
+  <si>
+    <t>low carbon</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>unequivocal</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>disruptive</t>
+  </si>
+  <si>
+    <t>imminent</t>
+  </si>
+  <si>
+    <t>resignation</t>
+  </si>
+  <si>
     <t>individual</t>
   </si>
   <si>
-    <t>committed</t>
-  </si>
-  <si>
-    <t>threat</t>
-  </si>
-  <si>
-    <t>extreme</t>
-  </si>
-  <si>
-    <t>investment</t>
-  </si>
-  <si>
-    <t>personal</t>
-  </si>
-  <si>
-    <t>disruptive</t>
-  </si>
-  <si>
-    <t>strife</t>
-  </si>
-  <si>
-    <t>long term</t>
-  </si>
-  <si>
-    <t>irreversible</t>
-  </si>
-  <si>
-    <t>nonpartisan</t>
-  </si>
-  <si>
-    <t>economic prosperity</t>
-  </si>
-  <si>
-    <t>cautious approach</t>
-  </si>
-  <si>
-    <t>consequence</t>
-  </si>
-  <si>
-    <t>footprint</t>
-  </si>
-  <si>
-    <t>reliable energy</t>
-  </si>
-  <si>
-    <t>impossible</t>
-  </si>
-  <si>
-    <t>total emissions</t>
-  </si>
-  <si>
-    <t>invent</t>
-  </si>
-  <si>
-    <t>take advantage</t>
-  </si>
-  <si>
-    <t>unavoidable</t>
-  </si>
-  <si>
-    <t>hinder</t>
-  </si>
-  <si>
-    <t>commitment</t>
+    <t>horizon</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>near future</t>
   </si>
   <si>
     <t>inevitable</t>
   </si>
   <si>
-    <t>exploited</t>
-  </si>
-  <si>
-    <t>fate</t>
-  </si>
-  <si>
-    <t>lowincome</t>
-  </si>
-  <si>
-    <t>adapt</t>
-  </si>
-  <si>
-    <t>overuse</t>
-  </si>
-  <si>
-    <t>cleaner fuels</t>
+    <t>invest</t>
+  </si>
+  <si>
+    <t>rush</t>
+  </si>
+  <si>
+    <t>adaptation</t>
   </si>
   <si>
     <t>doubt</t>
   </si>
   <si>
-    <t>catastrophe</t>
-  </si>
-  <si>
-    <t>natural gas</t>
-  </si>
-  <si>
-    <t>promised</t>
-  </si>
-  <si>
-    <t>mutually beneficial</t>
-  </si>
-  <si>
-    <t>fear</t>
-  </si>
-  <si>
-    <t>unimaginable</t>
-  </si>
-  <si>
-    <t>breakthrough</t>
-  </si>
-  <si>
-    <t>exploit</t>
-  </si>
-  <si>
-    <t>ambition</t>
-  </si>
-  <si>
-    <t>overburdened</t>
-  </si>
-  <si>
-    <t>competition</t>
-  </si>
-  <si>
-    <t>best interest</t>
-  </si>
-  <si>
-    <t>appetite</t>
-  </si>
-  <si>
-    <t>compromise</t>
-  </si>
-  <si>
-    <t>tragedy commons</t>
-  </si>
-  <si>
-    <t>consumer choice</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>living standards</t>
-  </si>
-  <si>
-    <t>low carbon</t>
-  </si>
-  <si>
-    <t>sequestration</t>
-  </si>
-  <si>
-    <t>burden</t>
-  </si>
-  <si>
-    <t>poor</t>
-  </si>
-  <si>
-    <t>fusion</t>
-  </si>
-  <si>
-    <t>renewable natural</t>
-  </si>
-  <si>
-    <t>regressive</t>
-  </si>
-  <si>
-    <t>voluntary</t>
-  </si>
-  <si>
     <t>lower carbon</t>
   </si>
   <si>
-    <t>adaptation</t>
-  </si>
-  <si>
-    <t>sacrifice</t>
-  </si>
-  <si>
-    <t>shared</t>
-  </si>
-  <si>
-    <t>compete</t>
-  </si>
-  <si>
-    <t>rush</t>
-  </si>
-  <si>
-    <t>insurmountable</t>
-  </si>
-  <si>
-    <t>grim</t>
-  </si>
-  <si>
-    <t>disproportionate</t>
-  </si>
-  <si>
-    <t>near future</t>
-  </si>
-  <si>
-    <t>marketplace</t>
-  </si>
-  <si>
-    <t>resignation</t>
-  </si>
-  <si>
-    <t>prescribe</t>
-  </si>
-  <si>
-    <t>promise</t>
-  </si>
-  <si>
-    <t>creator</t>
-  </si>
-  <si>
-    <t>costly</t>
-  </si>
-  <si>
-    <t>disruption</t>
-  </si>
-  <si>
-    <t>infeasible</t>
-  </si>
-  <si>
-    <t>negligible</t>
-  </si>
-  <si>
-    <t>affordable</t>
-  </si>
-  <si>
-    <t>overused</t>
-  </si>
-  <si>
-    <t>socioeconomic</t>
-  </si>
-  <si>
-    <t>uncertainty</t>
-  </si>
-  <si>
-    <t>incentive</t>
-  </si>
-  <si>
-    <t>unequivocal</t>
-  </si>
-  <si>
-    <t>energy needs</t>
-  </si>
-  <si>
-    <t>energy management</t>
-  </si>
-  <si>
-    <t>imminent</t>
-  </si>
-  <si>
-    <t>carbon intensity</t>
-  </si>
-  <si>
-    <t>carbon footprint</t>
-  </si>
-  <si>
-    <t>research development</t>
-  </si>
-  <si>
-    <t>invest</t>
-  </si>
-  <si>
-    <t>low income</t>
-  </si>
-  <si>
-    <t>exploiting</t>
-  </si>
-  <si>
-    <t>unfair</t>
-  </si>
-  <si>
-    <t>inflation</t>
-  </si>
-  <si>
-    <t>vulnerable</t>
-  </si>
-  <si>
-    <t>lost</t>
-  </si>
-  <si>
-    <t>share</t>
-  </si>
-  <si>
-    <t>private sector</t>
-  </si>
-  <si>
-    <t>innovation</t>
-  </si>
-  <si>
-    <t>horizon</t>
-  </si>
-  <si>
-    <t>volunteer</t>
-  </si>
-  <si>
-    <t>bipartisan</t>
-  </si>
-  <si>
-    <t>incentives</t>
+    <t>{'Individualism'}</t>
+  </si>
+  <si>
+    <t>{'Doomism'}</t>
+  </si>
+  <si>
+    <t>{'Tech_optimism'}</t>
+  </si>
+  <si>
+    <t>{'Free_rider'}</t>
+  </si>
+  <si>
+    <t>{'Social_justice'}</t>
+  </si>
+  <si>
+    <t>{'Carrots'}</t>
+  </si>
+  <si>
+    <t>{'Well_being'}</t>
   </si>
   <si>
     <t>{'Change_impossible'}</t>
   </si>
   <si>
+    <t>{'Whataboutism'}</t>
+  </si>
+  <si>
+    <t>{'Perfect_policy'}</t>
+  </si>
+  <si>
     <t>{'Talk_no_action'}</t>
   </si>
   <si>
-    <t>{'Individualism'}</t>
-  </si>
-  <si>
-    <t>{'Well_being'}</t>
-  </si>
-  <si>
-    <t>{'Doomism'}</t>
-  </si>
-  <si>
-    <t>{'Tech_optimism'}</t>
-  </si>
-  <si>
-    <t>{'Social_justice'}</t>
-  </si>
-  <si>
-    <t>{'Perfect_policy'}</t>
-  </si>
-  <si>
     <t>{'FF_solutionism'}</t>
   </si>
   <si>
-    <t>{'Whataboutism'}</t>
-  </si>
-  <si>
-    <t>{'Free_rider'}</t>
-  </si>
-  <si>
-    <t>{'Carrots'}</t>
-  </si>
-  <si>
-    <t>{'Free_rider', 'Carrots'}</t>
+    <t>{'Carrots', 'Free_rider'}</t>
   </si>
   <si>
     <t>{'Social_justice', 'Well_being'}</t>
   </si>
   <si>
-    <t>{'Free_rider', 'Social_justice', 'Carrots'}</t>
+    <t>{'Social_justice', 'Carrots', 'Free_rider'}</t>
   </si>
 </sst>
 </file>
@@ -768,13 +768,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.4432308849471093</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>109</v>
       </c>
       <c r="D2">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -782,13 +782,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-0.4424047452443152</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>110</v>
       </c>
       <c r="D3">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -796,13 +796,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.4420555844738485</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D4">
-        <v>190</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -810,13 +810,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-0.3887660374665793</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D5">
-        <v>261</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -824,13 +824,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-0.2692515226563703</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6">
-        <v>393</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -838,13 +838,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.1876325729197048</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7">
-        <v>367</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -852,13 +852,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.1477319125161749</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D8">
-        <v>94</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -866,13 +866,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-0.08532454921840424</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D9">
-        <v>440</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -880,13 +880,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>-0.02479582550875902</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D10">
-        <v>96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -897,10 +897,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D11">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -911,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -925,10 +925,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D13">
-        <v>67</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -939,10 +939,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D14">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -953,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D15">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -967,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -981,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -995,10 +995,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D18">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D19">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1023,10 +1023,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1037,10 +1037,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D21">
-        <v>41</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1051,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1065,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1079,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D24">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1093,10 +1093,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1107,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>629</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D27">
-        <v>629</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1138,7 +1138,7 @@
         <v>113</v>
       </c>
       <c r="D28">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1149,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1163,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D30">
-        <v>44</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1177,10 +1177,10 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D31">
-        <v>101</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1191,10 +1191,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D32">
-        <v>80</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1205,10 +1205,10 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D33">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1219,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1233,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D35">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1261,10 +1261,10 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D37">
-        <v>105</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1275,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D38">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1289,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1303,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D40">
-        <v>32</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1317,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1331,10 +1331,10 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D42">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1345,10 +1345,10 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D43">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1359,10 +1359,10 @@
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D44">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1373,10 +1373,10 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D45">
-        <v>6</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1387,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D46">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1401,10 +1401,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1415,10 +1415,10 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D48">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1429,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D49">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1443,10 +1443,10 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1457,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D52">
-        <v>136</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1485,10 +1485,10 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1499,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D54">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1513,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1527,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D56">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1541,10 +1541,10 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D57">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1555,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1569,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1583,10 +1583,10 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1597,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D61">
-        <v>79</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1611,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1625,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D63">
-        <v>44</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1639,10 +1639,10 @@
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D64">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1653,10 +1653,10 @@
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D65">
-        <v>229</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1667,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D66">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D67">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1695,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1709,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D69">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1723,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D70">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1737,10 +1737,10 @@
         <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1751,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D72">
-        <v>40</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1765,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D73">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1779,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1793,10 +1793,10 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D75">
-        <v>93</v>
+        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1807,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D76">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1821,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D77">
-        <v>49</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1835,10 +1835,10 @@
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D78">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>367</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1863,10 +1863,10 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D80">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1877,10 +1877,10 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D81">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1891,10 +1891,10 @@
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1905,10 +1905,10 @@
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D83">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1919,10 +1919,10 @@
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D84">
-        <v>17</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1933,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D85">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1947,10 +1947,10 @@
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D86">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1961,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D87">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1975,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D88">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1989,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D89">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2003,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2017,10 +2017,10 @@
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D91">
-        <v>21</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2031,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D92">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2045,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D93">
-        <v>151</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2073,10 +2073,10 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D95">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2087,10 +2087,10 @@
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D96">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2101,10 +2101,10 @@
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2112,13 +2112,13 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>0.01107190747934587</v>
+        <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D98">
-        <v>193</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2126,13 +2126,13 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>0.161138764811037</v>
+        <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D99">
-        <v>194</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2140,13 +2140,13 @@
         <v>102</v>
       </c>
       <c r="B100">
-        <v>0.2100830696858814</v>
+        <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D100">
-        <v>396</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2154,13 +2154,13 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>0.2180173262150243</v>
+        <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D101">
-        <v>75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2168,13 +2168,13 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>0.2337368045715202</v>
+        <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D102">
-        <v>188</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2182,13 +2182,13 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>0.3644207134070223</v>
+        <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D103">
-        <v>99</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2196,13 +2196,13 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>0.485639571212969</v>
+        <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D104">
-        <v>304</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2210,13 +2210,13 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>0.6078495832189693</v>
+        <v>0</v>
       </c>
       <c r="C105" t="s">
         <v>116</v>
       </c>
       <c r="D105">
-        <v>107</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2224,13 +2224,13 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>1.207540724375152</v>
+        <v>0</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
       </c>
       <c r="D106">
-        <v>227</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>